<commit_message>
Adjusted Payer, use Coverage for BankInformation Removed derived nl-core-patient profile Adjusted examples
</commit_message>
<xml_diff>
--- a/Mappings/Payer - STU3.xlsx
+++ b/Mappings/Payer - STU3.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Betaler" sheetId="1" r:id="rId1"/>
     <sheet name="VerzekeringssoortCodelijst" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterate="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="89">
   <si>
     <t xml:space="preserve"># </t>
   </si>
@@ -232,12 +232,6 @@
     <t>AT</t>
   </si>
   <si>
-    <t>Have to add a extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Patient (Derived nl-core-patient) / Coverage / Organization (Devrived nl-core-organization) </t>
-  </si>
-  <si>
     <t>nl-core-organization.telecom</t>
   </si>
   <si>
@@ -265,9 +259,6 @@
     <t>nl-core-organization.identifier.uzovi</t>
   </si>
   <si>
-    <t>Account</t>
-  </si>
-  <si>
     <t>.name</t>
   </si>
   <si>
@@ -278,6 +269,30 @@
   </si>
   <si>
     <t>.telecom</t>
+  </si>
+  <si>
+    <t>Coverage.payor.extension</t>
+  </si>
+  <si>
+    <t>.extension.BankName</t>
+  </si>
+  <si>
+    <t>.extension.Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added mapping fields </t>
+  </si>
+  <si>
+    <t>.extension.AccountNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coverage / Patient / RelatedPerson / Organization </t>
+  </si>
+  <si>
+    <t>extension</t>
+  </si>
+  <si>
+    <t>Need to place an invariant that makes identifier mandatory if Coverage.type = insurance or payor is referenced to an Organization</t>
   </si>
 </sst>
 </file>
@@ -649,38 +664,38 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -989,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1010,16 +1025,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
       <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1030,21 +1045,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="25.5">
+    <row r="2" spans="1:12" ht="15">
       <c r="A2" s="3"/>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
       <c r="K2" s="4" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="L2" s="4"/>
     </row>
@@ -1053,10 +1068,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6"/>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="43"/>
+      <c r="D3" s="42"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -1066,7 +1081,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="19"/>
       <c r="K3" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L3" s="10"/>
     </row>
@@ -1076,10 +1091,10 @@
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="20"/>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="35"/>
+      <c r="E4" s="34"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13" t="s">
@@ -1090,9 +1105,11 @@
         <v>6</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="L4" s="16"/>
+        <v>77</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="11">
@@ -1100,10 +1117,10 @@
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="20"/>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="35"/>
+      <c r="E5" s="34"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13" t="s">
@@ -1114,7 +1131,7 @@
         <v>8</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="L5" s="17"/>
     </row>
@@ -1124,10 +1141,10 @@
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="20"/>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="35"/>
+      <c r="E6" s="34"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13" t="s">
@@ -1138,7 +1155,7 @@
         <v>8</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="L6" s="17"/>
     </row>
@@ -1148,10 +1165,10 @@
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="20"/>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="35"/>
+      <c r="E7" s="34"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13" t="s">
@@ -1159,7 +1176,9 @@
       </c>
       <c r="I7" s="14"/>
       <c r="J7" s="19"/>
-      <c r="K7" s="15"/>
+      <c r="K7" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="L7" s="17"/>
     </row>
     <row r="8" spans="1:12">
@@ -1169,10 +1188,10 @@
       <c r="B8" s="12"/>
       <c r="C8" s="31"/>
       <c r="D8" s="31"/>
-      <c r="E8" s="44" t="s">
+      <c r="E8" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="44"/>
+      <c r="F8" s="35"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13" t="s">
         <v>31</v>
@@ -1182,10 +1201,10 @@
         <v>6</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1195,10 +1214,10 @@
       <c r="B9" s="12"/>
       <c r="C9" s="31"/>
       <c r="D9" s="31"/>
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="44"/>
+      <c r="F9" s="35"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13" t="s">
         <v>32</v>
@@ -1207,9 +1226,11 @@
       <c r="J9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="15"/>
+      <c r="K9" s="15" t="s">
+        <v>83</v>
+      </c>
       <c r="L9" s="17" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1219,10 +1240,10 @@
       <c r="B10" s="12"/>
       <c r="C10" s="31"/>
       <c r="D10" s="31"/>
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="44"/>
+      <c r="F10" s="35"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
         <v>33</v>
@@ -1231,9 +1252,11 @@
       <c r="J10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="15"/>
+      <c r="K10" s="15" t="s">
+        <v>85</v>
+      </c>
       <c r="L10" s="17" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1241,10 +1264,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="12"/>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="35"/>
+      <c r="D11" s="34"/>
       <c r="E11" s="32"/>
       <c r="F11" s="32"/>
       <c r="G11" s="13"/>
@@ -1262,10 +1285,10 @@
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="31"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="34"/>
       <c r="F12" s="32"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13" t="s">
@@ -1276,7 +1299,7 @@
         <v>43</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L12" s="17"/>
     </row>
@@ -1286,10 +1309,10 @@
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="31"/>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="35"/>
+      <c r="E13" s="34"/>
       <c r="F13" s="32"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13" t="s">
@@ -1300,20 +1323,20 @@
         <v>6</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L13" s="17"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" ht="25.5">
       <c r="A14" s="11">
         <v>12</v>
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="31"/>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="35"/>
+      <c r="E14" s="34"/>
       <c r="F14" s="32"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13" t="s">
@@ -1324,9 +1347,11 @@
         <v>6</v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="L14" s="17"/>
+        <v>71</v>
+      </c>
+      <c r="L14" s="17" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="11">
@@ -1334,10 +1359,10 @@
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="31"/>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="36"/>
+      <c r="E15" s="44"/>
       <c r="F15" s="32"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13" t="s">
@@ -1348,7 +1373,7 @@
         <v>8</v>
       </c>
       <c r="K15" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L15" s="17"/>
     </row>
@@ -1358,10 +1383,10 @@
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="31"/>
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="35"/>
+      <c r="E16" s="34"/>
       <c r="F16" s="32"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13" t="s">
@@ -1372,7 +1397,7 @@
         <v>8</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L16" s="17"/>
     </row>
@@ -1382,10 +1407,10 @@
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="31"/>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="35"/>
+      <c r="E17" s="34"/>
       <c r="F17" s="32"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13" t="s">
@@ -1403,10 +1428,10 @@
       <c r="B18" s="12"/>
       <c r="C18" s="31"/>
       <c r="D18" s="31"/>
-      <c r="E18" s="44" t="s">
+      <c r="E18" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="44"/>
+      <c r="F18" s="35"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13" t="s">
         <v>40</v>
@@ -1416,10 +1441,10 @@
         <v>7</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L18" s="33" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1429,10 +1454,10 @@
       <c r="B19" s="12"/>
       <c r="C19" s="31"/>
       <c r="D19" s="31"/>
-      <c r="E19" s="44" t="s">
+      <c r="E19" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="44"/>
+      <c r="F19" s="35"/>
       <c r="G19" s="13"/>
       <c r="H19" s="13" t="s">
         <v>41</v>
@@ -1442,7 +1467,7 @@
         <v>5</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L19" s="17"/>
     </row>
@@ -1453,10 +1478,10 @@
       <c r="B20" s="22"/>
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>
-      <c r="E20" s="34" t="s">
+      <c r="E20" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="34"/>
+      <c r="F20" s="43"/>
       <c r="G20" s="23"/>
       <c r="H20" s="23" t="s">
         <v>42</v>
@@ -1466,7 +1491,7 @@
         <v>5</v>
       </c>
       <c r="K20" s="25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L20" s="26"/>
     </row>
@@ -1504,16 +1529,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="D12:E12"/>
@@ -1524,6 +1539,16 @@
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>